<commit_message>
Added more detailed explanations to the answers
</commit_message>
<xml_diff>
--- a/study_guides/midterm_1_review/pipeline_2-wide-vliw_answer.xlsx
+++ b/study_guides/midterm_1_review/pipeline_2-wide-vliw_answer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrabb\Desktop\Wonsun Ahn\cs1541\CS1541_Fall2020\study_guides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wahn/Documents/teaching/cs1541/CS1541_Spring2022/study_guides/midterm_1_review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0997A8F1-D9C0-46CA-88F0-4682BE2E8B4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9161FA87-2452-8C49-8048-B9EFC68A206E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9225" yWindow="1065" windowWidth="19650" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20200" yWindow="5680" windowWidth="19660" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="23">
   <si>
     <t>Cycle</t>
   </si>
@@ -81,7 +81,19 @@
     <t>Assume split instruction and data memory, full data forwarding, and perfect branch prediction (with both BHT and BTB).</t>
   </si>
   <si>
-    <t>* Can be simulated using the 2-wide-opt.conf and midterm_1_review.tr trace.  The result is going be for an in-order superscalar but the only difference for a VLIW is that instead of the hazard detection unit inserting bubbles, the compiler schedules instructions so that there are no hazards.</t>
+    <t xml:space="preserve">First start by running "./five_stage_solution -c confs/2-wide-opt.conf -t midterm_1_review.tr ".  Write the generated schedule below. </t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID </t>
+  </si>
+  <si>
+    <t>The above result is  for an in-order superscalar but the only difference for a VLIW is that instead of the hazard detection unit inserting bubbles, the compiler schedules instructions so that there are no hazards.  Now write the compiler schedule based on the above schedule:</t>
   </si>
 </sst>
 </file>
@@ -137,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,6 +177,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,79 +470,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:Z12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="26" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="26" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -546,7 +570,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -626,25 +650,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -666,27 +680,17 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -706,27 +710,17 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -745,28 +739,18 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -784,28 +768,18 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -823,7 +797,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -831,21 +805,11 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="G10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -862,7 +826,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -890,37 +854,37 @@
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -948,235 +912,1006 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>2</v>
+      </c>
+      <c r="D14" s="8">
+        <v>3</v>
+      </c>
+      <c r="E14" s="8">
+        <v>4</v>
+      </c>
+      <c r="F14" s="8">
+        <v>5</v>
+      </c>
+      <c r="G14" s="8">
+        <v>6</v>
+      </c>
+      <c r="H14" s="8">
+        <v>7</v>
+      </c>
+      <c r="I14" s="8">
+        <v>8</v>
+      </c>
+      <c r="J14" s="8">
+        <v>9</v>
+      </c>
+      <c r="K14" s="8">
+        <v>10</v>
+      </c>
+      <c r="L14" s="8">
+        <v>11</v>
+      </c>
+      <c r="M14" s="8">
+        <v>12</v>
+      </c>
+      <c r="N14" s="8">
+        <v>13</v>
+      </c>
+      <c r="O14" s="8">
+        <v>14</v>
+      </c>
+      <c r="P14" s="8">
+        <v>15</v>
+      </c>
+      <c r="Q14" s="8">
         <v>16</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="R14" s="8">
+        <v>17</v>
+      </c>
+      <c r="S14" s="8">
+        <v>18</v>
+      </c>
+      <c r="T14" s="8">
+        <v>19</v>
+      </c>
+      <c r="U14" s="8">
+        <v>20</v>
+      </c>
+      <c r="V14" s="8">
+        <v>21</v>
+      </c>
+      <c r="W14" s="8">
+        <v>22</v>
+      </c>
+      <c r="X14" s="8">
+        <v>23</v>
+      </c>
+      <c r="Y14" s="8">
+        <v>24</v>
+      </c>
+      <c r="Z14" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>2</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>3</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>4</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+    </row>
+    <row r="22" spans="1:26" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8">
+        <v>2</v>
+      </c>
+      <c r="D24" s="8">
+        <v>3</v>
+      </c>
+      <c r="E24" s="8">
+        <v>4</v>
+      </c>
+      <c r="F24" s="8">
+        <v>5</v>
+      </c>
+      <c r="G24" s="8">
+        <v>6</v>
+      </c>
+      <c r="H24" s="8">
+        <v>7</v>
+      </c>
+      <c r="I24" s="8">
+        <v>8</v>
+      </c>
+      <c r="J24" s="8">
+        <v>9</v>
+      </c>
+      <c r="K24" s="8">
+        <v>10</v>
+      </c>
+      <c r="L24" s="8">
+        <v>11</v>
+      </c>
+      <c r="M24" s="8">
+        <v>12</v>
+      </c>
+      <c r="N24" s="8">
+        <v>13</v>
+      </c>
+      <c r="O24" s="8">
         <v>14</v>
       </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>5</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="P24" s="8">
+        <v>15</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>16</v>
+      </c>
+      <c r="R24" s="8">
+        <v>17</v>
+      </c>
+      <c r="S24" s="8">
+        <v>18</v>
+      </c>
+      <c r="T24" s="8">
+        <v>19</v>
+      </c>
+      <c r="U24" s="8">
+        <v>20</v>
+      </c>
+      <c r="V24" s="8">
+        <v>21</v>
+      </c>
+      <c r="W24" s="8">
+        <v>22</v>
+      </c>
+      <c r="X24" s="8">
+        <v>23</v>
+      </c>
+      <c r="Y24" s="8">
+        <v>24</v>
+      </c>
+      <c r="Z24" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="C25" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="D25" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="E25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
       <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="E27" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="6"/>
+      <c r="Z31" s="6"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="13"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>1</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>2</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>3</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>4</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>5</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>6</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>7</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>8</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>9</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>10</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="A12:Z12"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
+  <mergeCells count="27">
     <mergeCell ref="A1:Z1"/>
     <mergeCell ref="A2:Z2"/>
-    <mergeCell ref="A14:Z14"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="A32:Z32"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="A12:Z12"/>
+    <mergeCell ref="A22:Z22"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="B41:E41"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>